<commit_message>
wirte info to excel
</commit_message>
<xml_diff>
--- a/DHL_API_Sheet.xlsx
+++ b/DHL_API_Sheet.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\game\DHLfuncDev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA74ABAA-ABF8-4BBC-8C5C-2AEE66B125A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B2AD1B-541E-4512-A125-F27F38279914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="19575" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6675" yWindow="1905" windowWidth="19575" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="8" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Tracking Number</t>
   </si>
@@ -50,12 +37,21 @@
     <t>Destination</t>
   </si>
   <si>
-    <t>Events</t>
-  </si>
-  <si>
     <t>servicePoint</t>
   </si>
   <si>
+    <t>delivered</t>
+  </si>
+  <si>
+    <t>SEVILLA - SPAIN</t>
+  </si>
+  <si>
+    <t>MUNICH - GERMANY</t>
+  </si>
+  <si>
+    <t>{'timestamp': '2024-02-08T08:28:00', 'location': {'address': {'addressLocality': 'MUNICH - GERMANY'}}, 'description': 'Delivered', 'pieceIds': ['JD014600011333431260']}</t>
+  </si>
+  <si>
     <t>E.g</t>
   </si>
   <si>
@@ -78,6 +74,9 @@
   </si>
   <si>
     <t>"servicePoint":{"url":"http://www.dhl.es/en/country_profile.html"}</t>
+  </si>
+  <si>
+    <t>Events (newest)</t>
   </si>
 </sst>
 </file>
@@ -397,16 +396,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5F420CC-A300-4BAB-8035-5FEA91B94635}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -426,43 +428,55 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
         <v>6921406671</v>
       </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PLEASE USING XLSM TO OPEN
</commit_message>
<xml_diff>
--- a/DHL_API_Sheet.xlsx
+++ b/DHL_API_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\game\DHLfuncDev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1249B1-4BF6-499D-A71F-464475482E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B594DC66-4790-4527-9A74-F786C695F865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="1905" windowWidth="19575" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
add write excel with using time
</commit_message>
<xml_diff>
--- a/DHL_API_Sheet.xlsx
+++ b/DHL_API_Sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13575" windowWidth="23595" xWindow="2805" yWindow="1500"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13575" windowWidth="18660" xWindow="1005" yWindow="1035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt formatCode="[hh]:mm:ss" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="165"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -52,9 +55,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -393,10 +398,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:T16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:H2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -404,7 +409,9 @@
     <col customWidth="1" max="1" min="1" width="16"/>
     <col customWidth="1" max="4" min="4" width="23.5703125"/>
     <col customWidth="1" max="5" min="5" width="30.7109375"/>
-    <col customWidth="1" max="6" min="6" width="16.85546875"/>
+    <col customWidth="1" max="7" min="6" width="22.85546875"/>
+    <col customWidth="1" max="8" min="8" width="26"/>
+    <col customWidth="1" max="10" min="10" width="16.85546875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -430,15 +437,30 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
+          <t>send time</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
           <t>Destination</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>arrival time</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>duration time</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>Events (newest)</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>servicePoint</t>
         </is>
@@ -460,57 +482,223 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
+          <t>2024-02-07T17:25:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>MUNICH - GERMANY</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>{'timestamp': '2024-02-08T08:28:00', 'location': {'address': {'addressLocality': 'MUNICH - GERMANY'}}, 'description': 'Delivered', 'pieceIds': ['JD014600011333431260']}</t>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2024-02-08T08:28:00</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0.6270833333333333</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>8585095551</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>delivered</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MUNICH - GERMANY</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2024-02-26T19:09:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>CAMBRIDGE - UK</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2024-02-27T08:58:00</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0.5756944444444444</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4874299916</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>delivered</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>MUNICH - GERMANY</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2024-02-26T16:20:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>VERONA - ITALY</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2024-02-27T12:14:00</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0.8291666666666667</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3527880731</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>delivered</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>MUNICH - GERMANY</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2024-02-28T17:56:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>CAMBRIDGE - UK</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2024-03-01T08:47:00</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>1.61875</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>7177497666</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>delivered</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>MUNICH - GERMANY</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>45350.68472222222</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>VERONA - ITALY</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>45351.43194444444</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0.7472222222222222</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>89352111143</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6113737884</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>6691061322</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2685659756</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>6691061322</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>E.g</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>E.g</t>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>"id":"6921406671"</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>"service":"express"</t>
+        </is>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"status"{status: "delivered"} </t>
+        </is>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>"origin": {address:{"addresslocality": XXXX - SPAIN</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>"Destination": {address:{"addresslocality": XXXX - SPAIN</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>(the newest updata)  events[{0}]</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>"servicePoint":{"url":"http://www.dhl.es/en/country_profile.html"}</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>"id":"6921406671"</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>"service":"express"</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">"status"{status: "delivered"} </t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>"origin": {address:{"addresslocality": XXXX - SPAIN</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>"Destination": {address:{"addresslocality": XXXX - SPAIN</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>(the newest updata)  events[{0}]</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>"servicePoint":{"url":"http://www.dhl.es/en/country_profile.html"}</t>
-        </is>
+      <c r="A16" t="n">
+        <v>11111111111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>